<commit_message>
print and solve for unicut
</commit_message>
<xml_diff>
--- a/benders decomposition/k_results_decomposition.xlsx
+++ b/benders decomposition/k_results_decomposition.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="10">
   <si>
     <t>Budget</t>
   </si>
@@ -401,7 +401,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G24"/>
+  <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -458,7 +458,7 @@
         <v>2</v>
       </c>
       <c r="F3">
-        <v>4.320813200000089</v>
+        <v>10.62743169999885</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -478,7 +478,7 @@
         <v>2</v>
       </c>
       <c r="F4">
-        <v>4.397883499999921</v>
+        <v>11.21693030000461</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -498,7 +498,7 @@
         <v>2</v>
       </c>
       <c r="F5">
-        <v>4.273508600000014</v>
+        <v>10.892906699999</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -518,7 +518,7 @@
         <v>2</v>
       </c>
       <c r="F6">
-        <v>4.349770199999966</v>
+        <v>11.67338169999857</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -538,7 +538,7 @@
         <v>2</v>
       </c>
       <c r="F7">
-        <v>4.429327900000089</v>
+        <v>10.88322079999489</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -558,7 +558,7 @@
         <v>2</v>
       </c>
       <c r="F8">
-        <v>4.427034099999901</v>
+        <v>10.96941220000008</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -578,7 +578,7 @@
         <v>2</v>
       </c>
       <c r="F9">
-        <v>4.244944000000032</v>
+        <v>11.10764560000098</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -598,7 +598,7 @@
         <v>2</v>
       </c>
       <c r="F10">
-        <v>4.463868999999931</v>
+        <v>11.28365040000062</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -618,7 +618,7 @@
         <v>2</v>
       </c>
       <c r="F11">
-        <v>4.690548300000046</v>
+        <v>11.3287593999994</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -638,7 +638,7 @@
         <v>2</v>
       </c>
       <c r="F12">
-        <v>4.596865100000059</v>
+        <v>5.835396100002981</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -658,7 +658,7 @@
         <v>2</v>
       </c>
       <c r="F13">
-        <v>4.582729400000062</v>
+        <v>5.152236800000537</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -678,7 +678,7 @@
         <v>2</v>
       </c>
       <c r="F14">
-        <v>4.456991199999948</v>
+        <v>5.153378800001519</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -698,7 +698,7 @@
         <v>2</v>
       </c>
       <c r="F15">
-        <v>4.68010419999996</v>
+        <v>4.901795699996001</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -718,7 +718,7 @@
         <v>2</v>
       </c>
       <c r="F16">
-        <v>4.5748908999999</v>
+        <v>4.952405299998645</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -738,7 +738,7 @@
         <v>2</v>
       </c>
       <c r="F17">
-        <v>4.961695299999974</v>
+        <v>5.099446799998987</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -758,7 +758,7 @@
         <v>2</v>
       </c>
       <c r="F18">
-        <v>5.011641800000007</v>
+        <v>5.031342300004326</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -778,7 +778,7 @@
         <v>2</v>
       </c>
       <c r="F19">
-        <v>4.70192760000009</v>
+        <v>4.992929000000004</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -798,7 +798,7 @@
         <v>2</v>
       </c>
       <c r="F20">
-        <v>4.701554099999839</v>
+        <v>4.920939700001327</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -818,7 +818,7 @@
         <v>2</v>
       </c>
       <c r="F21">
-        <v>4.845873799999936</v>
+        <v>5.113470500000403</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -838,47 +838,7 @@
         <v>2</v>
       </c>
       <c r="F22">
-        <v>4.696559000000207</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6">
-      <c r="A23">
-        <v>900000000</v>
-      </c>
-      <c r="B23" t="s">
-        <v>7</v>
-      </c>
-      <c r="C23">
-        <v>-3794187190.648727</v>
-      </c>
-      <c r="D23">
-        <v>250</v>
-      </c>
-      <c r="E23">
-        <v>2</v>
-      </c>
-      <c r="F23">
-        <v>4.595809699999791</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6">
-      <c r="A24">
-        <v>900000000</v>
-      </c>
-      <c r="B24" t="s">
-        <v>8</v>
-      </c>
-      <c r="C24">
-        <v>-3794187190.648727</v>
-      </c>
-      <c r="D24">
-        <v>250</v>
-      </c>
-      <c r="E24">
-        <v>2</v>
-      </c>
-      <c r="F24">
-        <v>4.815540900000087</v>
+        <v>4.999486900000193</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added the simple moded without decomposition
</commit_message>
<xml_diff>
--- a/benders decomposition/k_results_decomposition.xlsx
+++ b/benders decomposition/k_results_decomposition.xlsx
@@ -458,7 +458,7 @@
         <v>2</v>
       </c>
       <c r="F3">
-        <v>10.62743169999885</v>
+        <v>10.95594069999788</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -478,7 +478,7 @@
         <v>2</v>
       </c>
       <c r="F4">
-        <v>11.21693030000461</v>
+        <v>11.30781500000012</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -498,7 +498,7 @@
         <v>2</v>
       </c>
       <c r="F5">
-        <v>10.892906699999</v>
+        <v>11.31903919999604</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -518,7 +518,7 @@
         <v>2</v>
       </c>
       <c r="F6">
-        <v>11.67338169999857</v>
+        <v>11.44202339999902</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -538,7 +538,7 @@
         <v>2</v>
       </c>
       <c r="F7">
-        <v>10.88322079999489</v>
+        <v>11.7871535000013</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -558,7 +558,7 @@
         <v>2</v>
       </c>
       <c r="F8">
-        <v>10.96941220000008</v>
+        <v>10.84841809999489</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -578,7 +578,7 @@
         <v>2</v>
       </c>
       <c r="F9">
-        <v>11.10764560000098</v>
+        <v>10.06526139999914</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -598,7 +598,7 @@
         <v>2</v>
       </c>
       <c r="F10">
-        <v>11.28365040000062</v>
+        <v>10.51989439999306</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -618,7 +618,7 @@
         <v>2</v>
       </c>
       <c r="F11">
-        <v>11.3287593999994</v>
+        <v>9.429674299994076</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -638,7 +638,7 @@
         <v>2</v>
       </c>
       <c r="F12">
-        <v>5.835396100002981</v>
+        <v>10.11985519999871</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -658,7 +658,7 @@
         <v>2</v>
       </c>
       <c r="F13">
-        <v>5.152236800000537</v>
+        <v>10.13611189999938</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -678,7 +678,7 @@
         <v>2</v>
       </c>
       <c r="F14">
-        <v>5.153378800001519</v>
+        <v>9.350660700001754</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -698,7 +698,7 @@
         <v>2</v>
       </c>
       <c r="F15">
-        <v>4.901795699996001</v>
+        <v>10.32756700000027</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -718,7 +718,7 @@
         <v>2</v>
       </c>
       <c r="F16">
-        <v>4.952405299998645</v>
+        <v>9.947236100000737</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -738,7 +738,7 @@
         <v>2</v>
       </c>
       <c r="F17">
-        <v>5.099446799998987</v>
+        <v>9.556730099997367</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -758,7 +758,7 @@
         <v>2</v>
       </c>
       <c r="F18">
-        <v>5.031342300004326</v>
+        <v>25.48973509999632</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -778,7 +778,7 @@
         <v>2</v>
       </c>
       <c r="F19">
-        <v>4.992929000000004</v>
+        <v>5.525759299998754</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -798,7 +798,7 @@
         <v>2</v>
       </c>
       <c r="F20">
-        <v>4.920939700001327</v>
+        <v>5.760017399996286</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -818,7 +818,7 @@
         <v>2</v>
       </c>
       <c r="F21">
-        <v>5.113470500000403</v>
+        <v>5.209805399994366</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -838,7 +838,7 @@
         <v>2</v>
       </c>
       <c r="F22">
-        <v>4.999486900000193</v>
+        <v>5.331813099997817</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed mistake in code
</commit_message>
<xml_diff>
--- a/benders decomposition/k_results_decomposition.xlsx
+++ b/benders decomposition/k_results_decomposition.xlsx
@@ -449,16 +449,16 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>-2550024868.748845</v>
+        <v>-2593924273.244156</v>
       </c>
       <c r="D3">
-        <v>3.362022592791824</v>
+        <v>12.0644725412605</v>
       </c>
       <c r="E3">
         <v>2</v>
       </c>
       <c r="F3">
-        <v>10.95594069999788</v>
+        <v>4.437355799993384</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -469,16 +469,16 @@
         <v>8</v>
       </c>
       <c r="C4">
-        <v>-2550024868.748845</v>
+        <v>-2593924273.244156</v>
       </c>
       <c r="D4">
-        <v>3.362022592791824</v>
+        <v>12.0644725412605</v>
       </c>
       <c r="E4">
         <v>2</v>
       </c>
       <c r="F4">
-        <v>11.30781500000012</v>
+        <v>4.064896199997747</v>
       </c>
     </row>
     <row r="5" spans="1:7">
@@ -489,16 +489,16 @@
         <v>7</v>
       </c>
       <c r="C5">
-        <v>-2558504710.092219</v>
+        <v>-2624353816.835186</v>
       </c>
       <c r="D5">
-        <v>5.043033889187735</v>
+        <v>18.09670881189074</v>
       </c>
       <c r="E5">
         <v>2</v>
       </c>
       <c r="F5">
-        <v>11.31903919999604</v>
+        <v>4.27215960000467</v>
       </c>
     </row>
     <row r="6" spans="1:7">
@@ -509,16 +509,16 @@
         <v>8</v>
       </c>
       <c r="C6">
-        <v>-2558504710.092219</v>
+        <v>-2624353816.835186</v>
       </c>
       <c r="D6">
-        <v>5.043033889187735</v>
+        <v>18.09670881189074</v>
       </c>
       <c r="E6">
         <v>2</v>
       </c>
       <c r="F6">
-        <v>11.44202339999902</v>
+        <v>4.232226200008881</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -529,16 +529,16 @@
         <v>7</v>
       </c>
       <c r="C7">
-        <v>-2702662012.929583</v>
+        <v>-3141656057.882689</v>
       </c>
       <c r="D7">
-        <v>33.62022592791823</v>
+        <v>120.644725412605</v>
       </c>
       <c r="E7">
         <v>2</v>
       </c>
       <c r="F7">
-        <v>11.7871535000013</v>
+        <v>4.536767899990082</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -549,16 +549,16 @@
         <v>8</v>
       </c>
       <c r="C8">
-        <v>-2702662012.929583</v>
+        <v>-3141656057.882689</v>
       </c>
       <c r="D8">
-        <v>33.62022592791823</v>
+        <v>120.644725412605</v>
       </c>
       <c r="E8">
         <v>2</v>
       </c>
       <c r="F8">
-        <v>10.84841809999489</v>
+        <v>4.135162399994442</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -569,16 +569,16 @@
         <v>7</v>
       </c>
       <c r="C9">
-        <v>-2872258839.79707</v>
+        <v>-3750246929.70328</v>
       </c>
       <c r="D9">
-        <v>67.24045185583647</v>
+        <v>241.2894508252099</v>
       </c>
       <c r="E9">
         <v>2</v>
       </c>
       <c r="F9">
-        <v>10.06526139999914</v>
+        <v>3.980953700011014</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -589,16 +589,16 @@
         <v>8</v>
       </c>
       <c r="C10">
-        <v>-2872258839.79707</v>
+        <v>-3750246929.703279</v>
       </c>
       <c r="D10">
-        <v>67.24045185583647</v>
+        <v>241.2894508252099</v>
       </c>
       <c r="E10">
         <v>2</v>
       </c>
       <c r="F10">
-        <v>10.51989439999306</v>
+        <v>4.252947700006189</v>
       </c>
     </row>
     <row r="11" spans="1:7">
@@ -609,16 +609,16 @@
         <v>7</v>
       </c>
       <c r="C11">
-        <v>-3041855666.664557</v>
+        <v>-3794187190.648727</v>
       </c>
       <c r="D11">
-        <v>100.8606777837547</v>
+        <v>250</v>
       </c>
       <c r="E11">
         <v>2</v>
       </c>
       <c r="F11">
-        <v>9.429674299994076</v>
+        <v>3.977119200004381</v>
       </c>
     </row>
     <row r="12" spans="1:7">
@@ -629,16 +629,16 @@
         <v>8</v>
       </c>
       <c r="C12">
-        <v>-3041855666.664557</v>
+        <v>-3794187190.648727</v>
       </c>
       <c r="D12">
-        <v>100.8606777837547</v>
+        <v>250</v>
       </c>
       <c r="E12">
         <v>2</v>
       </c>
       <c r="F12">
-        <v>10.11985519999871</v>
+        <v>4.197983900012332</v>
       </c>
     </row>
     <row r="13" spans="1:7">
@@ -649,16 +649,16 @@
         <v>7</v>
       </c>
       <c r="C13">
-        <v>-3211452493.532043</v>
+        <v>-3794187190.648727</v>
       </c>
       <c r="D13">
-        <v>134.4809037116729</v>
+        <v>250</v>
       </c>
       <c r="E13">
         <v>2</v>
       </c>
       <c r="F13">
-        <v>10.13611189999938</v>
+        <v>3.975355799993849</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -669,16 +669,16 @@
         <v>8</v>
       </c>
       <c r="C14">
-        <v>-3211452493.532043</v>
+        <v>-3794187190.648727</v>
       </c>
       <c r="D14">
-        <v>134.4809037116729</v>
+        <v>250</v>
       </c>
       <c r="E14">
         <v>2</v>
       </c>
       <c r="F14">
-        <v>9.350660700001754</v>
+        <v>4.294374000004609</v>
       </c>
     </row>
     <row r="15" spans="1:7">
@@ -689,16 +689,16 @@
         <v>7</v>
       </c>
       <c r="C15">
-        <v>-3381049320.39953</v>
+        <v>-3794187190.648727</v>
       </c>
       <c r="D15">
-        <v>168.1011296395912</v>
+        <v>250</v>
       </c>
       <c r="E15">
         <v>2</v>
       </c>
       <c r="F15">
-        <v>10.32756700000027</v>
+        <v>4.375703600002453</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -709,16 +709,16 @@
         <v>8</v>
       </c>
       <c r="C16">
-        <v>-3381049320.39953</v>
+        <v>-3794187190.648727</v>
       </c>
       <c r="D16">
-        <v>168.1011296395912</v>
+        <v>250</v>
       </c>
       <c r="E16">
         <v>2</v>
       </c>
       <c r="F16">
-        <v>9.947236100000737</v>
+        <v>4.057205500008422</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -729,16 +729,16 @@
         <v>7</v>
       </c>
       <c r="C17">
-        <v>-3550646147.267016</v>
+        <v>-3794187190.648727</v>
       </c>
       <c r="D17">
-        <v>201.7213555675094</v>
+        <v>250</v>
       </c>
       <c r="E17">
         <v>2</v>
       </c>
       <c r="F17">
-        <v>9.556730099997367</v>
+        <v>4.173780500001158</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -749,16 +749,16 @@
         <v>8</v>
       </c>
       <c r="C18">
-        <v>-3550646147.267016</v>
+        <v>-3794187190.648727</v>
       </c>
       <c r="D18">
-        <v>201.7213555675094</v>
+        <v>250</v>
       </c>
       <c r="E18">
         <v>2</v>
       </c>
       <c r="F18">
-        <v>25.48973509999632</v>
+        <v>4.184106500004418</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -769,16 +769,16 @@
         <v>7</v>
       </c>
       <c r="C19">
-        <v>-3720242974.134504</v>
+        <v>-3794187190.648727</v>
       </c>
       <c r="D19">
-        <v>235.3415814954276</v>
+        <v>250</v>
       </c>
       <c r="E19">
         <v>2</v>
       </c>
       <c r="F19">
-        <v>5.525759299998754</v>
+        <v>4.062346799997613</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -789,16 +789,16 @@
         <v>8</v>
       </c>
       <c r="C20">
-        <v>-3720242974.134505</v>
+        <v>-3794187190.648727</v>
       </c>
       <c r="D20">
-        <v>235.3415814954276</v>
+        <v>250</v>
       </c>
       <c r="E20">
         <v>2</v>
       </c>
       <c r="F20">
-        <v>5.760017399996286</v>
+        <v>4.317703799999435</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -818,7 +818,7 @@
         <v>2</v>
       </c>
       <c r="F21">
-        <v>5.209805399994366</v>
+        <v>4.023150499997428</v>
       </c>
     </row>
     <row r="22" spans="1:6">
@@ -838,7 +838,7 @@
         <v>2</v>
       </c>
       <c r="F22">
-        <v>5.331813099997817</v>
+        <v>4.262797599993064</v>
       </c>
     </row>
   </sheetData>

</xml_diff>